<commit_message>
Added surgery, manner of death and Time From Pregnancy fields in the documentation. Updated the sample files csv and xlsx
</commit_message>
<xml_diff>
--- a/en/docs/sample.xlsx
+++ b/en/docs/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\projects\electronic-death-certificate-format-tabular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai\Documents\GitHub\doris\en\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3C3DCD-3B67-45EA-8C95-ACFE542EA167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FBFBBC-DBC1-487C-90D4-39AE19BC1797}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30825" yWindow="-105" windowWidth="30930" windowHeight="16890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
   <si>
     <t>CertificateKey</t>
   </si>
@@ -212,6 +212,15 @@
   </si>
   <si>
     <t>CauseOfDeathTextE</t>
+  </si>
+  <si>
+    <t>SurgeryWasPerformed</t>
+  </si>
+  <si>
+    <t>MannerOfDeath</t>
+  </si>
+  <si>
+    <t>MaternalDeathTimeFromPregnancy</t>
   </si>
 </sst>
 </file>
@@ -1080,21 +1089,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH5"/>
+  <dimension ref="A1:AK5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.77734375" customWidth="1"/>
-    <col min="10" max="10" width="22.21875" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1186,19 +1195,28 @@
         <v>62</v>
       </c>
       <c r="AE1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG1" t="s">
         <v>24</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI1" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1206,7 +1224,7 @@
         <v>28</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -1235,14 +1253,8 @@
       <c r="U2" t="s">
         <v>37</v>
       </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1250,7 +1262,7 @@
         <v>28</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
         <v>38</v>
@@ -1285,14 +1297,8 @@
       <c r="AC3" t="s">
         <v>48</v>
       </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1300,7 +1306,7 @@
         <v>28</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
         <v>49</v>
@@ -1329,14 +1335,8 @@
       <c r="AC4" t="s">
         <v>57</v>
       </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>28</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
         <v>49</v>
@@ -1372,12 +1372,6 @@
       </c>
       <c r="AC5" t="s">
         <v>57</v>
-      </c>
-      <c r="AE5">
-        <v>0</v>
-      </c>
-      <c r="AF5">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to Doris documentation
</commit_message>
<xml_diff>
--- a/en/docs/sample.xlsx
+++ b/en/docs/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai\Documents\GitHub\doris\en\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\gitrepos\Docs\doris\en\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FBFBBC-DBC1-487C-90D4-39AE19BC1797}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7309BD6D-12F0-4DD7-AB04-380AFAF87569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30825" yWindow="-105" windowWidth="30930" windowHeight="16890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
@@ -40,57 +40,36 @@
     <t>DateDeath</t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>CauseOfDeathA</t>
-  </si>
-  <si>
     <t>CauseOfDeathURIA</t>
   </si>
   <si>
     <t>IntervalA</t>
   </si>
   <si>
-    <t>CauseOfDeathB</t>
-  </si>
-  <si>
     <t>CauseOfDeathURIB</t>
   </si>
   <si>
     <t>IntervalB</t>
   </si>
   <si>
-    <t>CauseOfDeathC</t>
-  </si>
-  <si>
     <t>CauseOfDeathURIC</t>
   </si>
   <si>
     <t>IntervalC</t>
   </si>
   <si>
-    <t>CauseOfDeathD</t>
-  </si>
-  <si>
     <t>CauseOfDeathURID</t>
   </si>
   <si>
     <t>IntervalD</t>
   </si>
   <si>
-    <t>CauseOfDeathE</t>
-  </si>
-  <si>
     <t>CauseOfDeathURIE</t>
   </si>
   <si>
     <t>IntervalE</t>
   </si>
   <si>
-    <t>CauseOfDeathPart2</t>
-  </si>
-  <si>
     <t>CauseOfDeathURIPart2</t>
   </si>
   <si>
@@ -221,6 +200,27 @@
   </si>
   <si>
     <t>MaternalDeathTimeFromPregnancy</t>
+  </si>
+  <si>
+    <t>EstimatedAge</t>
+  </si>
+  <si>
+    <t>CauseOfDeathCodeA</t>
+  </si>
+  <si>
+    <t>CauseOfDeathCodeB</t>
+  </si>
+  <si>
+    <t>CauseOfDeathCodeC</t>
+  </si>
+  <si>
+    <t>CauseOfDeathCodeD</t>
+  </si>
+  <si>
+    <t>CauseOfDeathCodeE</t>
+  </si>
+  <si>
+    <t>CauseOfDeathCodePart2</t>
   </si>
 </sst>
 </file>
@@ -793,9 +793,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -833,7 +833,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -939,7 +939,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1081,7 +1081,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1091,19 +1091,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="10" max="10" width="22.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1123,255 +1121,255 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" t="s">
+        <v>54</v>
+      </c>
+      <c r="W1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF1" t="s">
         <v>58</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="AG1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH1" t="s">
         <v>59</v>
       </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="AI1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AJ1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AK1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" t="s">
         <v>29</v>
       </c>
-      <c r="H2" t="s">
+      <c r="U2" t="s">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" t="s">
         <v>38</v>
       </c>
-      <c r="H3" t="s">
+      <c r="U3" t="s">
         <v>39</v>
       </c>
-      <c r="I3" t="s">
+      <c r="AB3" t="s">
         <v>40</v>
       </c>
-      <c r="L3" t="s">
+      <c r="AC3" t="s">
         <v>41</v>
       </c>
-      <c r="M3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T3" t="s">
-        <v>45</v>
-      </c>
-      <c r="U3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>48</v>
-      </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB4" t="s">
         <v>49</v>
       </c>
-      <c r="H4" t="s">
+      <c r="AC4" t="s">
         <v>50</v>
       </c>
-      <c r="I4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" t="s">
-        <v>52</v>
-      </c>
-      <c r="M4" t="s">
-        <v>53</v>
-      </c>
-      <c r="P4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>57</v>
-      </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" t="s">
+      <c r="AC5" t="s">
         <v>50</v>
-      </c>
-      <c r="I5" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" t="s">
-        <v>52</v>
-      </c>
-      <c r="M5" t="s">
-        <v>53</v>
-      </c>
-      <c r="P5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed the URIs in excel and CSV samples
</commit_message>
<xml_diff>
--- a/en/docs/sample.xlsx
+++ b/en/docs/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\gitrepos\Docs\doris\en\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\GitRepos\Docs\doris\en\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7309BD6D-12F0-4DD7-AB04-380AFAF87569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9F6FC8-4D3A-4EFA-8140-1D71818AD3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
@@ -94,87 +94,48 @@
     <t>BA41.Z</t>
   </si>
   <si>
-    <t>http://id.who.int/icd/entity/1334938734/mms/unspecified</t>
-  </si>
-  <si>
     <t>2C25.Z</t>
   </si>
   <si>
-    <t>http://id.who.int/icd/entity/316539081/mms/unspecified</t>
-  </si>
-  <si>
     <t>2E2Z</t>
   </si>
   <si>
-    <t>http://id.who.int/icd/entity/1917052637/mms/unspecified</t>
-  </si>
-  <si>
     <t>BA00.Z</t>
   </si>
   <si>
-    <t>http://id.who.int/icd/entity/761947693/mms/unspecified</t>
-  </si>
-  <si>
     <t>P40Y</t>
   </si>
   <si>
     <t>BD1Z</t>
   </si>
   <si>
-    <t>http://id.who.int/icd/entity/1458683894/mms/unspecified</t>
-  </si>
-  <si>
     <t>BB40</t>
   </si>
   <si>
-    <t>http://id.who.int/icd/entity/512128824</t>
-  </si>
-  <si>
     <t>BB6Z</t>
   </si>
   <si>
-    <t>http://id.who.int/icd/entity/1997348476/mms/unspecified</t>
-  </si>
-  <si>
     <t>BC20.1</t>
   </si>
   <si>
-    <t>http://id.who.int/icd/entity/770085732</t>
-  </si>
-  <si>
     <t>6C40.2Z</t>
   </si>
   <si>
-    <t>http://id.who.int/icd/entity/1580466198/mms/unspecified</t>
-  </si>
-  <si>
     <t>P0Y</t>
   </si>
   <si>
     <t>MG40.0</t>
   </si>
   <si>
-    <t>http://id.who.int/icd/entity/1974956233</t>
-  </si>
-  <si>
     <t>LA8Z</t>
   </si>
   <si>
-    <t>http://id.who.int/icd/entity/2004408087/mms/unspecified</t>
-  </si>
-  <si>
     <t>LB30.9</t>
   </si>
   <si>
-    <t>http://id.who.int/icd/entity/1178642763</t>
-  </si>
-  <si>
     <t>KA21.4Z</t>
   </si>
   <si>
-    <t>http://id.who.int/icd/entity/1726201225/mms/unspecified</t>
-  </si>
-  <si>
     <t>CauseOfDeathTextA</t>
   </si>
   <si>
@@ -221,13 +182,52 @@
   </si>
   <si>
     <t>CauseOfDeathCodePart2</t>
+  </si>
+  <si>
+    <t>http://id.who.int/icd/release/11/mms/1334938734/unspecified</t>
+  </si>
+  <si>
+    <t>http://id.who.int/icd/release/11/mms/1458683894/unspecified</t>
+  </si>
+  <si>
+    <t>http://id.who.int/icd/release/11/mms/1974956233</t>
+  </si>
+  <si>
+    <t>http://id.who.int/icd/release/11/mms/316539081/unspecified</t>
+  </si>
+  <si>
+    <t>http://id.who.int/icd/release/11/mms/512128824</t>
+  </si>
+  <si>
+    <t>http://id.who.int/icd/release/11/mms/2004408087/unspecified</t>
+  </si>
+  <si>
+    <t>http://id.who.int/icd/release/11/mms/1917052637/unspecified</t>
+  </si>
+  <si>
+    <t>http://id.who.int/icd/release/11/mms/1997348476/unspecified</t>
+  </si>
+  <si>
+    <t>http://id.who.int/icd/release/11/mms/1178642763</t>
+  </si>
+  <si>
+    <t>http://id.who.int/icd/release/11/mms/761947693/unspecified</t>
+  </si>
+  <si>
+    <t>http://id.who.int/icd/release/11/mms/770085732</t>
+  </si>
+  <si>
+    <t>http://id.who.int/icd/release/11/mms/1580466198/unspecified</t>
+  </si>
+  <si>
+    <t>http://id.who.int/icd/release/11/mms/1726201225/unspecified</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +358,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -660,7 +668,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -703,11 +711,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -741,6 +751,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -793,9 +804,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -833,7 +844,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -939,7 +950,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1081,7 +1092,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1091,17 +1102,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AC6" sqref="AC6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="8" max="8" width="15.26953125" customWidth="1"/>
-    <col min="9" max="9" width="23" customWidth="1"/>
-    <col min="10" max="10" width="22.26953125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="58.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" customWidth="1"/>
+    <col min="13" max="13" width="67.42578125" customWidth="1"/>
+    <col min="17" max="17" width="69.140625" customWidth="1"/>
+    <col min="21" max="21" width="57.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="71.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1121,88 +1139,88 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
       </c>
       <c r="N1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="O1" t="s">
         <v>9</v>
       </c>
       <c r="P1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="Q1" t="s">
         <v>10</v>
       </c>
       <c r="R1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="S1" t="s">
         <v>11</v>
       </c>
       <c r="T1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="U1" t="s">
         <v>12</v>
       </c>
       <c r="V1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="W1" t="s">
         <v>13</v>
       </c>
       <c r="X1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="Y1" t="s">
         <v>14</v>
       </c>
       <c r="Z1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="AA1" t="s">
         <v>15</v>
       </c>
       <c r="AB1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="AC1" t="s">
         <v>16</v>
       </c>
       <c r="AD1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="AE1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="AF1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="AG1" t="s">
         <v>17</v>
       </c>
       <c r="AH1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="AI1" t="s">
         <v>18</v>
@@ -1214,7 +1232,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1230,29 +1248,29 @@
       <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T2" t="s">
         <v>26</v>
       </c>
-      <c r="P2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2" t="s">
-        <v>30</v>
+      <c r="U2" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1263,40 +1281,40 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
+      <c r="U3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB3" t="s">
         <v>32</v>
       </c>
-      <c r="I3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>41</v>
+      <c r="AC3" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1307,34 +1325,34 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="L4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" t="s">
-        <v>46</v>
+        <v>35</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="P4" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>48</v>
+        <v>36</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="AB4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1345,34 +1363,53 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="L5" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" t="s">
-        <v>46</v>
+        <v>35</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="P5" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>48</v>
+        <v>36</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="AB5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{3793BF20-722C-41DC-A45D-1115D5D67E79}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{D684A2D0-730D-48D6-A6CC-844102C72AEC}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{C9D2F1CD-396A-4C67-8298-46F2DA888E5F}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{210B168C-7EE4-43B1-BB55-AE6BBD2D4B2A}"/>
+    <hyperlink ref="M2" r:id="rId5" xr:uid="{47972767-7DF0-4289-99A5-8D76506C5ACB}"/>
+    <hyperlink ref="M3" r:id="rId6" xr:uid="{C8C2D2DB-6499-4CFB-A945-7210A7B24B7C}"/>
+    <hyperlink ref="M4" r:id="rId7" xr:uid="{E2C8D3E6-074F-4569-A547-82D8D11B2FC7}"/>
+    <hyperlink ref="M5" r:id="rId8" xr:uid="{F167847D-950D-4F7F-83AE-0615A3A192CB}"/>
+    <hyperlink ref="Q2" r:id="rId9" xr:uid="{823448DA-AAAA-4B65-A7E9-F7BB185A5371}"/>
+    <hyperlink ref="Q3" r:id="rId10" xr:uid="{1E5F0CC2-4E89-4137-B4F5-677DF3C42FF5}"/>
+    <hyperlink ref="Q4" r:id="rId11" xr:uid="{CD84E9B7-7D3A-4FA6-BE11-07AE845FC862}"/>
+    <hyperlink ref="Q5" r:id="rId12" xr:uid="{3DCACB45-289C-497A-B12A-FFDBACB9C4B8}"/>
+    <hyperlink ref="U2" r:id="rId13" xr:uid="{43197E93-4EB6-45FB-92F5-E5B0016CBB46}"/>
+    <hyperlink ref="U3" r:id="rId14" xr:uid="{63221CA9-420C-4929-B556-E1460023C230}"/>
+    <hyperlink ref="AC3" r:id="rId15" xr:uid="{E006E1F5-0601-4CD7-B285-C2C1E9E2261A}"/>
+    <hyperlink ref="AC4" r:id="rId16" xr:uid="{FC264C60-7F4D-4D6F-92DE-03E8B3CD7EA1}"/>
+    <hyperlink ref="AC5" r:id="rId17" xr:uid="{C6DDE82B-475C-4060-8E7C-9362C550BEE9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>